<commit_message>
Fin de la création des unités
</commit_message>
<xml_diff>
--- a/Liste des unités.xlsx
+++ b/Liste des unités.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julot/Documents/EMA/2A/Conception orienté objet Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julot/food-crops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC8214C-D0A8-D742-9693-A098D09F27DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3BBE8E-57A9-0045-84CE-67A2B219EB35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B4013500-C21C-7049-A287-ED89132C25B6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{B4013500-C21C-7049-A287-ED89132C25B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Ratio</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>Million Bushel</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>acre</t>
@@ -570,9 +567,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1BA0B9-536D-8144-B12A-DC4E65AB0B16}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="225" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,13 +604,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>22</v>
@@ -653,7 +650,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -667,14 +664,14 @@
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -688,7 +685,7 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -698,7 +695,7 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -708,7 +705,7 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -718,7 +715,7 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -728,7 +725,7 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -745,10 +742,18 @@
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="F13" s="7" t="s">
         <v>11</v>
       </c>
@@ -757,13 +762,13 @@
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>29</v>
+      <c r="B14" s="3">
+        <v>1</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
-        <v>29</v>
+      <c r="E14" s="3">
+        <v>2</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>0</v>
@@ -774,11 +779,11 @@
         <v>20</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>29</v>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="8" t="s">
@@ -789,11 +794,11 @@
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>29</v>
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -804,11 +809,11 @@
         <v>7</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>29</v>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
@@ -818,11 +823,11 @@
         <v>19</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>29</v>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="1"/>
@@ -832,11 +837,11 @@
         <v>10</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>29</v>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="1"/>
@@ -847,11 +852,11 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>29</v>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -861,11 +866,11 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>29</v>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2</v>
       </c>
       <c r="F21" s="1"/>
     </row>

</xml_diff>